<commit_message>
Changes to CKinetics.m and modelgen.m that need to be merged into new git exit
</commit_message>
<xml_diff>
--- a/KineticModel/Kotte2014/Kotte2014.xlsx
+++ b/KineticModel/Kotte2014/Kotte2014.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>Enzymes</t>
   </si>
@@ -129,9 +129,6 @@
     <t>GLUX</t>
   </si>
   <si>
-    <t>GLUY</t>
-  </si>
-  <si>
     <t>ENZC</t>
   </si>
   <si>
@@ -160,6 +157,21 @@
   </si>
   <si>
     <t>enz1[c]</t>
+  </si>
+  <si>
+    <t>ACt2r</t>
+  </si>
+  <si>
+    <t>FDPt2r</t>
+  </si>
+  <si>
+    <t>FBP</t>
+  </si>
+  <si>
+    <t>2 fdp[c]</t>
+  </si>
+  <si>
+    <t>4 pep[c]</t>
   </si>
 </sst>
 </file>
@@ -238,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -247,6 +259,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,7 +563,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:U7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -647,12 +662,15 @@
       <c r="J2" s="4">
         <v>0</v>
       </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
       <c r="M2" s="5">
         <v>14.285714285714301</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S2" t="s">
         <v>21</v>
@@ -680,13 +698,16 @@
       <c r="J3">
         <v>0</v>
       </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
       <c r="O3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -704,10 +725,10 @@
         <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>35</v>
-      </c>
-      <c r="P4" t="s">
-        <v>28</v>
+        <v>34</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="R4">
         <v>0.1</v>
@@ -715,7 +736,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>26</v>
@@ -733,15 +754,18 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="P5" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="R5">
         <v>0.45</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -754,8 +778,11 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -787,12 +814,12 @@
         <v>18</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2">
         <v>0.1</v>
@@ -816,7 +843,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -824,7 +851,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -832,7 +859,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
Need to check fluxEnvelope.m
</commit_message>
<xml_diff>
--- a/KineticModel/Kotte2014/Kotte2014.xlsx
+++ b/KineticModel/Kotte2014/Kotte2014.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>Enzymes</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>4 pep[c]</t>
+  </si>
+  <si>
+    <t>ENZt2r</t>
+  </si>
+  <si>
+    <t>enz1[c] &lt;==&gt;</t>
   </si>
 </sst>
 </file>
@@ -561,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:U7"/>
+      <selection sqref="A1:U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,6 +579,8 @@
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="20" max="20" width="12.28515625" customWidth="1"/>
+    <col min="21" max="21" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
@@ -791,6 +799,23 @@
         <v>1</v>
       </c>
       <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
functional MATCONT for Kotte model w/ flux envelopes
</commit_message>
<xml_diff>
--- a/KineticModel/Kotte2014/Kotte2014.xlsx
+++ b/KineticModel/Kotte2014/Kotte2014.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>Enzymes</t>
   </si>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>enz1[c] &lt;==&gt;</t>
+  </si>
+  <si>
+    <t>ENZtr</t>
+  </si>
+  <si>
+    <t>enz[c] &lt;==&gt;</t>
   </si>
 </sst>
 </file>
@@ -567,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:U8"/>
+      <selection activeCell="C8" sqref="C8:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,6 +822,23 @@
         <v>1</v>
       </c>
       <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working CNA code with Kotte model
</commit_message>
<xml_diff>
--- a/KineticModel/Kotte2014/Kotte2014.xlsx
+++ b/KineticModel/Kotte2014/Kotte2014.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>Enzymes</t>
   </si>
@@ -114,9 +114,6 @@
     <t>pep[c] ---&gt; fdp[c]</t>
   </si>
   <si>
-    <t>fdp[c] ---&gt; fdp[e]</t>
-  </si>
-  <si>
     <t>enz1[c] ---&gt; enz[c]</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
     <t>ac[e] &lt;==&gt;</t>
   </si>
   <si>
-    <t>fdp[e] &lt;==&gt;</t>
-  </si>
-  <si>
     <t>fdp[e]</t>
   </si>
   <si>
@@ -165,9 +159,6 @@
     <t>FDPt2r</t>
   </si>
   <si>
-    <t>FBP</t>
-  </si>
-  <si>
     <t>2 fdp[c]</t>
   </si>
   <si>
@@ -177,13 +168,52 @@
     <t>ENZt2r</t>
   </si>
   <si>
-    <t>enz1[c] &lt;==&gt;</t>
-  </si>
-  <si>
     <t>ENZtr</t>
   </si>
   <si>
-    <t>enz[c] &lt;==&gt;</t>
+    <t>PEPt2r</t>
+  </si>
+  <si>
+    <t>EC_Biomass</t>
+  </si>
+  <si>
+    <t>pep[c] &lt;==&gt; pep[e]</t>
+  </si>
+  <si>
+    <t>PEPex</t>
+  </si>
+  <si>
+    <t>pep[e] &lt;==&gt;</t>
+  </si>
+  <si>
+    <t>ENZ1ex</t>
+  </si>
+  <si>
+    <t>ENZex</t>
+  </si>
+  <si>
+    <t>enz1[c] &lt;==&gt; enz1[e]</t>
+  </si>
+  <si>
+    <t>enz[c] &lt;==&gt; enz[e]</t>
+  </si>
+  <si>
+    <t>fdp[c] ---&gt; bm[c]</t>
+  </si>
+  <si>
+    <t>FDex</t>
+  </si>
+  <si>
+    <t>bm[e] &lt;==&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enz1[e] &lt;==&gt; </t>
+  </si>
+  <si>
+    <t>enz[e] &lt;==&gt;</t>
+  </si>
+  <si>
+    <t>bm[c] ---&gt; bm[e]</t>
   </si>
 </sst>
 </file>
@@ -573,14 +603,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C9"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
@@ -684,7 +716,7 @@
       </c>
       <c r="N2" s="3"/>
       <c r="O2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S2" t="s">
         <v>21</v>
@@ -698,7 +730,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -716,15 +748,15 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="E4">
         <v>-30.5</v>
@@ -739,10 +771,10 @@
         <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="R4">
         <v>0.1</v>
@@ -750,10 +782,10 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5">
         <v>-30.5</v>
@@ -768,7 +800,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="P5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="R5">
         <v>0.45</v>
@@ -776,10 +808,10 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -793,10 +825,10 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -810,10 +842,10 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -827,19 +859,77 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>47</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>48</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -862,12 +952,12 @@
         <v>18</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>0.1</v>
@@ -875,7 +965,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="7">
         <v>1E-3</v>
@@ -883,7 +973,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="7">
         <v>10</v>
@@ -891,7 +981,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -899,7 +989,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -907,7 +997,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
CMCS with CNA - working versin
</commit_message>
<xml_diff>
--- a/KineticModel/Kotte2014/Kotte2014.xlsx
+++ b/KineticModel/Kotte2014/Kotte2014.xlsx
@@ -156,9 +156,6 @@
     <t>ACt2r</t>
   </si>
   <si>
-    <t>FDPt2r</t>
-  </si>
-  <si>
     <t>2 fdp[c]</t>
   </si>
   <si>
@@ -177,9 +174,6 @@
     <t>EC_Biomass</t>
   </si>
   <si>
-    <t>pep[c] &lt;==&gt; pep[e]</t>
-  </si>
-  <si>
     <t>PEPex</t>
   </si>
   <si>
@@ -195,15 +189,9 @@
     <t>enz1[c] &lt;==&gt; enz1[e]</t>
   </si>
   <si>
-    <t>enz[c] &lt;==&gt; enz[e]</t>
-  </si>
-  <si>
     <t>fdp[c] ---&gt; bm[c]</t>
   </si>
   <si>
-    <t>FDex</t>
-  </si>
-  <si>
     <t>bm[e] &lt;==&gt;</t>
   </si>
   <si>
@@ -214,6 +202,18 @@
   </si>
   <si>
     <t>bm[c] ---&gt; bm[e]</t>
+  </si>
+  <si>
+    <t>pep[c] ---&gt; pep[e]</t>
+  </si>
+  <si>
+    <t>enz[c] ---&gt; enz[e]</t>
+  </si>
+  <si>
+    <t>bmt2r</t>
+  </si>
+  <si>
+    <t>bmex</t>
   </si>
 </sst>
 </file>
@@ -606,7 +606,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,10 +753,10 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E4">
         <v>-30.5</v>
@@ -774,7 +774,7 @@
         <v>33</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R4">
         <v>0.1</v>
@@ -800,7 +800,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="P5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R5">
         <v>0.45</v>
@@ -825,10 +825,10 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -842,10 +842,10 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -859,10 +859,10 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -876,10 +876,10 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -893,10 +893,10 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -910,26 +910,26 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Parameter sampling for Kottemodel - initial commit
</commit_message>
<xml_diff>
--- a/KineticModel/Kotte2014/Kotte2014.xlsx
+++ b/KineticModel/Kotte2014/Kotte2014.xlsx
@@ -605,9 +605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -915,6 +913,9 @@
       <c r="C12" t="s">
         <v>52</v>
       </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -923,6 +924,9 @@
       <c r="C13" t="s">
         <v>53</v>
       </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -931,9 +935,13 @@
       <c r="C14" t="s">
         <v>51</v>
       </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changes to add enz[c] as a regulator
</commit_message>
<xml_diff>
--- a/KineticModel/Kotte2014/Kotte2014.xlsx
+++ b/KineticModel/Kotte2014/Kotte2014.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
   <si>
     <t>Enzymes</t>
   </si>
@@ -605,7 +605,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:U14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -715,6 +717,9 @@
       <c r="N2" s="3"/>
       <c r="O2" t="s">
         <v>33</v>
+      </c>
+      <c r="P2" t="s">
+        <v>32</v>
       </c>
       <c r="S2" t="s">
         <v>21</v>

</xml_diff>